<commit_message>
fix converter for answers
also shorten tab name for DGA formulaire
</commit_message>
<xml_diff>
--- a/tools/DGA/Formulaire-SDI-SecNum-2216.xlsx
+++ b/tools/DGA/Formulaire-SDI-SecNum-2216.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/imanabshirali/Desktop/stage MAi/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/DGA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E2FC00-F4BD-254D-800B-8AFEA8AB7C77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E81AA0-AA3C-7444-B0E4-1B5271F7BFB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="17520" activeTab="1" xr2:uid="{777C2D61-8F41-684C-B0E9-3CB5A9BB2C0B}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="17520" xr2:uid="{777C2D61-8F41-684C-B0E9-3CB5A9BB2C0B}"/>
   </bookViews>
   <sheets>
     <sheet name="library_content" sheetId="1" r:id="rId1"/>
-    <sheet name="Formulaire-SDI-SecNum-2216" sheetId="3" r:id="rId2"/>
-    <sheet name="answers" sheetId="2" r:id="rId3"/>
+    <sheet name="Formulaire" sheetId="3" r:id="rId2"/>
+    <sheet name="réponses" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="203">
   <si>
     <t>assessable</t>
   </si>
@@ -525,9 +525,6 @@
     <t>Annotation</t>
   </si>
   <si>
-    <t>Formulaire-SDI-SecNum-2216</t>
-  </si>
-  <si>
     <t>typical_evidence</t>
   </si>
   <si>
@@ -831,6 +828,12 @@
   <si>
     <t xml:space="preserve">La messagerie est sécurisée par des équipements ou des services permettant de réduire drastiquement le nombre et la portée des messages malveillants.
 </t>
+  </si>
+  <si>
+    <t>Formulaire</t>
+  </si>
+  <si>
+    <t>réponses</t>
   </si>
 </sst>
 </file>
@@ -1069,7 +1072,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1387,8 +1390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7858AAA4-43A5-D54D-90D1-1E3D474B5994}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="200" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1403,7 +1406,7 @@
         <v>37</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C1" s="9"/>
     </row>
@@ -1430,7 +1433,7 @@
         <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1447,7 +1450,7 @@
         <v>42</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C6" s="9"/>
     </row>
@@ -1483,7 +1486,7 @@
         <v>47</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C10" s="9"/>
     </row>
@@ -1492,7 +1495,7 @@
         <v>48</v>
       </c>
       <c r="B11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C11" s="9"/>
     </row>
@@ -1510,7 +1513,7 @@
         <v>50</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C13" s="9"/>
     </row>
@@ -1519,7 +1522,7 @@
         <v>51</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>127</v>
+        <v>201</v>
       </c>
       <c r="C14" s="19" t="s">
         <v>52</v>
@@ -1530,7 +1533,7 @@
         <v>51</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>65</v>
+        <v>202</v>
       </c>
       <c r="C15" s="19" t="s">
         <v>65</v>
@@ -1545,7 +1548,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9D5AD9A-7258-874C-9314-54460A1C2E84}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
+    <sheetView zoomScale="94" workbookViewId="0">
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
@@ -1587,7 +1590,7 @@
         <v>126</v>
       </c>
       <c r="I1" s="22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="64" x14ac:dyDescent="0.2">
@@ -1598,7 +1601,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>8</v>
@@ -1607,7 +1610,7 @@
         <v>13</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G2" t="s">
         <v>66</v>
@@ -1627,22 +1630,22 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G3" t="s">
         <v>67</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I3" s="14" t="s">
         <v>104</v>
@@ -1656,7 +1659,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>10</v>
@@ -1665,7 +1668,7 @@
         <v>36</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G4" t="s">
         <v>68</v>
@@ -1685,7 +1688,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>11</v>
@@ -1694,13 +1697,13 @@
         <v>35</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G5" t="s">
         <v>69</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I5" s="14" t="s">
         <v>106</v>
@@ -1714,7 +1717,7 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>12</v>
@@ -1723,7 +1726,7 @@
         <v>34</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G6" t="s">
         <v>70</v>
@@ -1743,22 +1746,22 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G7" t="s">
         <v>71</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I7" s="14" t="s">
         <v>108</v>
@@ -1772,22 +1775,22 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G8" t="s">
         <v>72</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I8" s="12" t="s">
         <v>109</v>
@@ -1801,22 +1804,22 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G9" t="s">
         <v>73</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>110</v>
@@ -1830,7 +1833,7 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>17</v>
@@ -1839,7 +1842,7 @@
         <v>33</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G10" t="s">
         <v>74</v>
@@ -1859,16 +1862,16 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G11" t="s">
         <v>75</v>
@@ -1888,16 +1891,16 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>18</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G12" t="s">
         <v>76</v>
@@ -1917,25 +1920,25 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G13" t="s">
         <v>77</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="119" x14ac:dyDescent="0.2">
@@ -1946,22 +1949,22 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>20</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G14" t="s">
         <v>78</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>114</v>
@@ -1975,22 +1978,22 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>20</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G15" t="s">
         <v>79</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I15" s="14" t="s">
         <v>115</v>
@@ -2004,22 +2007,22 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>21</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G16" t="s">
         <v>80</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I16" s="20" t="s">
         <v>116</v>
@@ -2033,7 +2036,7 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>22</v>
@@ -2042,7 +2045,7 @@
         <v>32</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G17" t="s">
         <v>81</v>
@@ -2062,7 +2065,7 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>23</v>
@@ -2071,7 +2074,7 @@
         <v>31</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G18" t="s">
         <v>82</v>
@@ -2091,7 +2094,7 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>23</v>
@@ -2100,7 +2103,7 @@
         <v>30</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G19" t="s">
         <v>83</v>
@@ -2120,7 +2123,7 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>24</v>
@@ -2129,7 +2132,7 @@
         <v>29</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G20" t="s">
         <v>84</v>
@@ -2149,7 +2152,7 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D21" s="27" t="s">
         <v>25</v>
@@ -2158,13 +2161,13 @@
         <v>28</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G21" t="s">
         <v>85</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I21" s="14" t="s">
         <v>121</v>
@@ -2178,7 +2181,7 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>26</v>
@@ -2187,7 +2190,7 @@
         <v>27</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G22" t="s">
         <v>86</v>
@@ -2260,7 +2263,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="96" x14ac:dyDescent="0.2">
@@ -2282,7 +2285,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="144" x14ac:dyDescent="0.2">
@@ -2315,7 +2318,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="112" x14ac:dyDescent="0.2">
@@ -2370,7 +2373,7 @@
         <v>7</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="80" x14ac:dyDescent="0.2">
@@ -2381,7 +2384,7 @@
         <v>7</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="112" x14ac:dyDescent="0.2">
@@ -2392,10 +2395,10 @@
         <v>7</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>81</v>
       </c>
@@ -2403,7 +2406,7 @@
         <v>7</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="112" x14ac:dyDescent="0.2">
@@ -2414,7 +2417,7 @@
         <v>7</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="112" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
feat(lib): tooling for new Excel format (#1963)
* Create convert_v1_to_v2.py

* fix converter for answers

also shorten tab name for DGA formulaire

* create_library

New version for convert_library, based on v2 format for Excel

* DGA questionnaire OK

* Update convert_v1_to_v2.py

copy colors

* matrix OK

* Update convert_v1_to_v2.py

manage mappings correctly

* manage mappings

works for ccb mapping
</commit_message>
<xml_diff>
--- a/tools/DGA/Formulaire-SDI-SecNum-2216.xlsx
+++ b/tools/DGA/Formulaire-SDI-SecNum-2216.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/imanabshirali/Desktop/stage MAi/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/DGA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E2FC00-F4BD-254D-800B-8AFEA8AB7C77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E81AA0-AA3C-7444-B0E4-1B5271F7BFB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="17520" activeTab="1" xr2:uid="{777C2D61-8F41-684C-B0E9-3CB5A9BB2C0B}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="17520" xr2:uid="{777C2D61-8F41-684C-B0E9-3CB5A9BB2C0B}"/>
   </bookViews>
   <sheets>
     <sheet name="library_content" sheetId="1" r:id="rId1"/>
-    <sheet name="Formulaire-SDI-SecNum-2216" sheetId="3" r:id="rId2"/>
-    <sheet name="answers" sheetId="2" r:id="rId3"/>
+    <sheet name="Formulaire" sheetId="3" r:id="rId2"/>
+    <sheet name="réponses" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="203">
   <si>
     <t>assessable</t>
   </si>
@@ -525,9 +525,6 @@
     <t>Annotation</t>
   </si>
   <si>
-    <t>Formulaire-SDI-SecNum-2216</t>
-  </si>
-  <si>
     <t>typical_evidence</t>
   </si>
   <si>
@@ -831,6 +828,12 @@
   <si>
     <t xml:space="preserve">La messagerie est sécurisée par des équipements ou des services permettant de réduire drastiquement le nombre et la portée des messages malveillants.
 </t>
+  </si>
+  <si>
+    <t>Formulaire</t>
+  </si>
+  <si>
+    <t>réponses</t>
   </si>
 </sst>
 </file>
@@ -1069,7 +1072,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1387,8 +1390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7858AAA4-43A5-D54D-90D1-1E3D474B5994}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="200" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1403,7 +1406,7 @@
         <v>37</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C1" s="9"/>
     </row>
@@ -1430,7 +1433,7 @@
         <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1447,7 +1450,7 @@
         <v>42</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C6" s="9"/>
     </row>
@@ -1483,7 +1486,7 @@
         <v>47</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C10" s="9"/>
     </row>
@@ -1492,7 +1495,7 @@
         <v>48</v>
       </c>
       <c r="B11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C11" s="9"/>
     </row>
@@ -1510,7 +1513,7 @@
         <v>50</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C13" s="9"/>
     </row>
@@ -1519,7 +1522,7 @@
         <v>51</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>127</v>
+        <v>201</v>
       </c>
       <c r="C14" s="19" t="s">
         <v>52</v>
@@ -1530,7 +1533,7 @@
         <v>51</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>65</v>
+        <v>202</v>
       </c>
       <c r="C15" s="19" t="s">
         <v>65</v>
@@ -1545,7 +1548,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9D5AD9A-7258-874C-9314-54460A1C2E84}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
+    <sheetView zoomScale="94" workbookViewId="0">
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
@@ -1587,7 +1590,7 @@
         <v>126</v>
       </c>
       <c r="I1" s="22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="64" x14ac:dyDescent="0.2">
@@ -1598,7 +1601,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>8</v>
@@ -1607,7 +1610,7 @@
         <v>13</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G2" t="s">
         <v>66</v>
@@ -1627,22 +1630,22 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G3" t="s">
         <v>67</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I3" s="14" t="s">
         <v>104</v>
@@ -1656,7 +1659,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>10</v>
@@ -1665,7 +1668,7 @@
         <v>36</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G4" t="s">
         <v>68</v>
@@ -1685,7 +1688,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>11</v>
@@ -1694,13 +1697,13 @@
         <v>35</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G5" t="s">
         <v>69</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I5" s="14" t="s">
         <v>106</v>
@@ -1714,7 +1717,7 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>12</v>
@@ -1723,7 +1726,7 @@
         <v>34</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G6" t="s">
         <v>70</v>
@@ -1743,22 +1746,22 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G7" t="s">
         <v>71</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I7" s="14" t="s">
         <v>108</v>
@@ -1772,22 +1775,22 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G8" t="s">
         <v>72</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I8" s="12" t="s">
         <v>109</v>
@@ -1801,22 +1804,22 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G9" t="s">
         <v>73</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>110</v>
@@ -1830,7 +1833,7 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>17</v>
@@ -1839,7 +1842,7 @@
         <v>33</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G10" t="s">
         <v>74</v>
@@ -1859,16 +1862,16 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G11" t="s">
         <v>75</v>
@@ -1888,16 +1891,16 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>18</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G12" t="s">
         <v>76</v>
@@ -1917,25 +1920,25 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G13" t="s">
         <v>77</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="119" x14ac:dyDescent="0.2">
@@ -1946,22 +1949,22 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>20</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G14" t="s">
         <v>78</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>114</v>
@@ -1975,22 +1978,22 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>20</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G15" t="s">
         <v>79</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I15" s="14" t="s">
         <v>115</v>
@@ -2004,22 +2007,22 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>21</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G16" t="s">
         <v>80</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I16" s="20" t="s">
         <v>116</v>
@@ -2033,7 +2036,7 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>22</v>
@@ -2042,7 +2045,7 @@
         <v>32</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G17" t="s">
         <v>81</v>
@@ -2062,7 +2065,7 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>23</v>
@@ -2071,7 +2074,7 @@
         <v>31</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G18" t="s">
         <v>82</v>
@@ -2091,7 +2094,7 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>23</v>
@@ -2100,7 +2103,7 @@
         <v>30</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G19" t="s">
         <v>83</v>
@@ -2120,7 +2123,7 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>24</v>
@@ -2129,7 +2132,7 @@
         <v>29</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G20" t="s">
         <v>84</v>
@@ -2149,7 +2152,7 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D21" s="27" t="s">
         <v>25</v>
@@ -2158,13 +2161,13 @@
         <v>28</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G21" t="s">
         <v>85</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I21" s="14" t="s">
         <v>121</v>
@@ -2178,7 +2181,7 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>26</v>
@@ -2187,7 +2190,7 @@
         <v>27</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G22" t="s">
         <v>86</v>
@@ -2260,7 +2263,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="96" x14ac:dyDescent="0.2">
@@ -2282,7 +2285,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="144" x14ac:dyDescent="0.2">
@@ -2315,7 +2318,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="112" x14ac:dyDescent="0.2">
@@ -2370,7 +2373,7 @@
         <v>7</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="80" x14ac:dyDescent="0.2">
@@ -2381,7 +2384,7 @@
         <v>7</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="112" x14ac:dyDescent="0.2">
@@ -2392,10 +2395,10 @@
         <v>7</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>81</v>
       </c>
@@ -2403,7 +2406,7 @@
         <v>7</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="112" x14ac:dyDescent="0.2">
@@ -2414,7 +2417,7 @@
         <v>7</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="112" x14ac:dyDescent="0.2">

</xml_diff>